<commit_message>
build the big table in optimization.tex
</commit_message>
<xml_diff>
--- a/other/STT-RAM-Metrics.xlsx
+++ b/other/STT-RAM-Metrics.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="11055" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="11055" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>Write Pulse (ns)</t>
   </si>
@@ -83,6 +84,27 @@
   <si>
     <t>Minimum Write Latency</t>
   </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>WL</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>Bigtable</t>
+  </si>
 </sst>
 </file>
 
@@ -141,9 +163,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11389942454376301"/>
-          <c:y val="5.2124536157118352E-2"/>
+          <c:y val="5.2124536157118366E-2"/>
           <c:w val="0.83550020786408863"/>
-          <c:h val="0.77094636057816779"/>
+          <c:h val="0.7709463605781679"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -529,11 +551,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="63904768"/>
-        <c:axId val="65196032"/>
+        <c:axId val="103923712"/>
+        <c:axId val="103926016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63904768"/>
+        <c:axId val="103923712"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -561,12 +583,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65196032"/>
+        <c:crossAx val="103926016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65196032"/>
+        <c:axId val="103926016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -606,7 +628,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="63904768"/>
+        <c:crossAx val="103923712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -618,8 +640,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.3583724569640084E-2"/>
-          <c:y val="9.4258665942619391E-2"/>
-          <c:w val="0.66472613458529028"/>
+          <c:y val="9.4258665942619432E-2"/>
+          <c:w val="0.66472613458529051"/>
           <c:h val="0.2321723232871753"/>
         </c:manualLayout>
       </c:layout>
@@ -638,7 +660,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -659,7 +681,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947998"/>
+          <c:h val="0.7704993994394802"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1045,11 +1067,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="165488512"/>
-        <c:axId val="165568512"/>
+        <c:axId val="104572416"/>
+        <c:axId val="104574336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165488512"/>
+        <c:axId val="104572416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1072,18 +1094,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165568512"/>
+        <c:crossAx val="104574336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165568512"/>
+        <c:axId val="104574336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -1107,12 +1128,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165488512"/>
+        <c:crossAx val="104572416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -1126,8 +1146,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.14141459590278491"/>
           <c:y val="9.2892839404204494E-2"/>
-          <c:w val="0.63690166001977133"/>
-          <c:h val="0.22826898361842757"/>
+          <c:w val="0.63690166001977155"/>
+          <c:h val="0.22826898361842762"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1150,7 +1170,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1168,10 +1188,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15430118110236254"/>
+          <c:x val="0.1543011811023626"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.80727006780402455"/>
-          <c:h val="0.77049939943947998"/>
+          <c:h val="0.7704993994394802"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1557,11 +1577,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="165956224"/>
-        <c:axId val="165987840"/>
+        <c:axId val="104608512"/>
+        <c:axId val="104610432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165956224"/>
+        <c:axId val="104608512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1584,18 +1604,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165987840"/>
+        <c:crossAx val="104610432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165987840"/>
+        <c:axId val="104610432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130"/>
@@ -1619,12 +1638,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165956224"/>
+        <c:crossAx val="104608512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -1636,10 +1654,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355239"/>
+          <c:x val="0.35808141629355245"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.59480200011494744"/>
-          <c:h val="0.22826898361842757"/>
+          <c:w val="0.59480200011494733"/>
+          <c:h val="0.22826898361842762"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -1662,7 +1680,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2069,11 +2087,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="168001536"/>
-        <c:axId val="168003456"/>
+        <c:axId val="104643968"/>
+        <c:axId val="104666624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="168001536"/>
+        <c:axId val="104643968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2096,18 +2114,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168003456"/>
+        <c:crossAx val="104666624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="168003456"/>
+        <c:axId val="104666624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -2131,12 +2148,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="168001536"/>
+        <c:crossAx val="104643968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -2149,9 +2165,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.3665412807854978"/>
-          <c:y val="3.044194157075869E-2"/>
-          <c:w val="0.59480200011494722"/>
-          <c:h val="0.22826898361842768"/>
+          <c:y val="3.0441941570758697E-2"/>
+          <c:w val="0.5948020001149471"/>
+          <c:h val="0.22826898361842773"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2174,7 +2190,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2195,7 +2211,7 @@
           <c:x val="0.1437743056986987"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.81759574555798331"/>
-          <c:h val="0.77049939943947998"/>
+          <c:h val="0.7704993994394802"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2581,11 +2597,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="179150848"/>
-        <c:axId val="179153536"/>
+        <c:axId val="104738176"/>
+        <c:axId val="104744448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179150848"/>
+        <c:axId val="104738176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2608,18 +2624,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179153536"/>
+        <c:crossAx val="104744448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179153536"/>
+        <c:axId val="104744448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2651,12 +2666,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179150848"/>
+        <c:crossAx val="104738176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -2668,10 +2682,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26085903324584464"/>
-          <c:y val="0.15896612261215706"/>
-          <c:w val="0.59480200011494744"/>
-          <c:h val="0.24592897742086889"/>
+          <c:x val="0.26085903324584475"/>
+          <c:y val="0.15896612261215709"/>
+          <c:w val="0.59480200011494733"/>
+          <c:h val="0.24592897742086892"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -2694,7 +2708,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2715,7 +2729,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.81685870516185477"/>
-          <c:h val="0.68311193658932201"/>
+          <c:h val="0.68311193658932212"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2922,11 +2936,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140175616"/>
-        <c:axId val="152302720"/>
+        <c:axId val="106911232"/>
+        <c:axId val="106926080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140175616"/>
+        <c:axId val="106911232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2968,14 +2982,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152302720"/>
+        <c:crossAx val="106926080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152302720"/>
+        <c:axId val="106926080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8"/>
@@ -3016,7 +3030,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140175616"/>
+        <c:crossAx val="106911232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3028,10 +3042,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12865252012989897"/>
+          <c:x val="0.12865252012989895"/>
           <c:y val="6.8676713424067018E-2"/>
           <c:w val="0.56322033898305079"/>
-          <c:h val="0.21338478385566048"/>
+          <c:h val="0.21338478385566051"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3049,7 +3063,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3070,7 +3084,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947798"/>
+          <c:h val="0.77049939943947821"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3456,11 +3470,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="68666112"/>
-        <c:axId val="71613824"/>
+        <c:axId val="103759232"/>
+        <c:axId val="103773696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="68666112"/>
+        <c:axId val="103759232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3487,13 +3501,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71613824"/>
+        <c:crossAx val="103773696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71613824"/>
+        <c:axId val="103773696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3528,7 +3542,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68666112"/>
+        <c:crossAx val="103759232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3539,10 +3553,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355184"/>
+          <c:x val="0.35808141629355189"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.59480200011494855"/>
-          <c:h val="0.22826898361842723"/>
+          <c:w val="0.59480200011494844"/>
+          <c:h val="0.22826898361842726"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -3560,7 +3574,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3581,7 +3595,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.7704993994394792"/>
+          <c:h val="0.77049939943947943"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3967,11 +3981,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91034752"/>
-        <c:axId val="91500544"/>
+        <c:axId val="103950976"/>
+        <c:axId val="103961344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91034752"/>
+        <c:axId val="103950976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -3998,13 +4012,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91500544"/>
+        <c:crossAx val="103961344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91500544"/>
+        <c:axId val="103961344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -4032,7 +4046,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91034752"/>
+        <c:crossAx val="103950976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -4044,10 +4058,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355217"/>
+          <c:x val="0.35808141629355222"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.59480200011494788"/>
-          <c:h val="0.22826898361842746"/>
+          <c:w val="0.59480200011494777"/>
+          <c:h val="0.22826898361842748"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -4070,7 +4084,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4091,7 +4105,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947965"/>
+          <c:h val="0.77049939943947976"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4477,11 +4491,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94588928"/>
-        <c:axId val="94591232"/>
+        <c:axId val="103987072"/>
+        <c:axId val="103997440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94588928"/>
+        <c:axId val="103987072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -4508,13 +4522,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94591232"/>
+        <c:crossAx val="103997440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94591232"/>
+        <c:axId val="103997440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -4542,7 +4556,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94588928"/>
+        <c:crossAx val="103987072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
@@ -4554,10 +4568,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14141469816272997"/>
-          <c:y val="9.3292869641294976E-2"/>
+          <c:x val="0.14141469816273003"/>
+          <c:y val="9.3292869641295004E-2"/>
           <c:w val="0.5364687226596675"/>
-          <c:h val="0.22826898361842751"/>
+          <c:h val="0.22826898361842754"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -4580,7 +4594,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4601,7 +4615,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947965"/>
+          <c:h val="0.77049939943947976"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4987,11 +5001,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="94871936"/>
-        <c:axId val="94874624"/>
+        <c:axId val="104051840"/>
+        <c:axId val="104053760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94871936"/>
+        <c:axId val="104051840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -5018,13 +5032,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94874624"/>
+        <c:crossAx val="104053760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94874624"/>
+        <c:axId val="104053760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="130"/>
@@ -5052,7 +5066,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94871936"/>
+        <c:crossAx val="104051840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -5064,10 +5078,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355228"/>
+          <c:x val="0.35808141629355233"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.59480200011494766"/>
-          <c:h val="0.22826898361842751"/>
+          <c:w val="0.59480200011494755"/>
+          <c:h val="0.22826898361842754"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -5090,7 +5104,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5111,7 +5125,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947998"/>
+          <c:h val="0.7704993994394802"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5497,11 +5511,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="114604288"/>
-        <c:axId val="117469952"/>
+        <c:axId val="104079744"/>
+        <c:axId val="104081664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="114604288"/>
+        <c:axId val="104079744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -5536,13 +5550,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117469952"/>
+        <c:crossAx val="104081664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="117469952"/>
+        <c:axId val="104081664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="150"/>
@@ -5570,7 +5584,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114604288"/>
+        <c:crossAx val="104079744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -5582,10 +5596,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.33863692038495247"/>
-          <c:y val="9.3292869641294976E-2"/>
-          <c:w val="0.59480200011494744"/>
-          <c:h val="0.22826898361842757"/>
+          <c:x val="0.33863692038495258"/>
+          <c:y val="9.3292869641295004E-2"/>
+          <c:w val="0.59480200011494733"/>
+          <c:h val="0.22826898361842762"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -5608,7 +5622,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5629,7 +5643,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947965"/>
+          <c:h val="0.77049939943947976"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6015,11 +6029,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="128314368"/>
-        <c:axId val="139709056"/>
+        <c:axId val="104123776"/>
+        <c:axId val="104134144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="128314368"/>
+        <c:axId val="104123776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -6046,13 +6060,13 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139709056"/>
+        <c:crossAx val="104134144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139709056"/>
+        <c:axId val="104134144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6088,7 +6102,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128314368"/>
+        <c:crossAx val="104123776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -6100,10 +6114,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808136482939662"/>
+          <c:x val="0.35808136482939668"/>
           <c:y val="0.17662620297462819"/>
-          <c:w val="0.59480200011494766"/>
-          <c:h val="0.22826898361842751"/>
+          <c:w val="0.59480200011494755"/>
+          <c:h val="0.22826898361842754"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -6126,7 +6140,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6147,7 +6161,7 @@
           <c:x val="0.12930796150481189"/>
           <c:y val="5.1400554097404488E-2"/>
           <c:w val="0.83504786539363762"/>
-          <c:h val="0.77049939943947843"/>
+          <c:h val="0.77049939943947865"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6533,11 +6547,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="164424320"/>
-        <c:axId val="164639488"/>
+        <c:axId val="104483456"/>
+        <c:axId val="104497920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164424320"/>
+        <c:axId val="104483456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -6560,18 +6574,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164639488"/>
+        <c:crossAx val="104497920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164639488"/>
+        <c:axId val="104497920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -6602,12 +6615,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164424320"/>
+        <c:crossAx val="104483456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6618,10 +6630,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355195"/>
+          <c:x val="0.358081416293552"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.59480200011494833"/>
-          <c:h val="0.22826898361842729"/>
+          <c:w val="0.59480200011494821"/>
+          <c:h val="0.22826898361842732"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -6644,7 +6656,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6662,10 +6674,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15079213009600981"/>
+          <c:x val="0.15079213009600986"/>
           <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.81067878264564242"/>
-          <c:h val="0.77049939943947876"/>
+          <c:w val="0.81067878264564253"/>
+          <c:h val="0.77049939943947898"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -7051,11 +7063,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="165128064"/>
-        <c:axId val="165135872"/>
+        <c:axId val="104527744"/>
+        <c:axId val="104542208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165128064"/>
+        <c:axId val="104527744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -7078,18 +7090,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165135872"/>
+        <c:crossAx val="104542208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165135872"/>
+        <c:axId val="104542208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -7113,12 +7124,11 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165128064"/>
+        <c:crossAx val="104527744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -7130,10 +7140,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35808141629355206"/>
+          <c:x val="0.35808141629355211"/>
           <c:y val="6.5515014013078923E-2"/>
-          <c:w val="0.5948020001149481"/>
-          <c:h val="0.22826898361842737"/>
+          <c:w val="0.59480200011494799"/>
+          <c:h val="0.22826898361842743"/>
         </c:manualLayout>
       </c:layout>
       <c:txPr>
@@ -7156,7 +7166,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9720,7 +9730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -9930,4 +9940,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:8">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>3.06</v>
+      </c>
+      <c r="D4">
+        <v>10.7</v>
+      </c>
+      <c r="E4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F4">
+        <v>5.66</v>
+      </c>
+      <c r="G4">
+        <v>6.22</v>
+      </c>
+      <c r="H4">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>21.8</v>
+      </c>
+      <c r="D5">
+        <v>3.7</v>
+      </c>
+      <c r="E5">
+        <v>4.92</v>
+      </c>
+      <c r="F5">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="G5">
+        <v>9.57</v>
+      </c>
+      <c r="H5">
+        <v>9.91</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D6">
+        <v>13.9</v>
+      </c>
+      <c r="E6">
+        <v>4.01</v>
+      </c>
+      <c r="F6">
+        <v>15.9</v>
+      </c>
+      <c r="G6">
+        <v>11.3</v>
+      </c>
+      <c r="H6">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D7">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.316</v>
+      </c>
+      <c r="F7">
+        <v>0.105</v>
+      </c>
+      <c r="G7">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.27900000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D8">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.309</v>
+      </c>
+      <c r="F8">
+        <v>0.193</v>
+      </c>
+      <c r="G8">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>1.01</v>
+      </c>
+      <c r="D9">
+        <v>3.53</v>
+      </c>
+      <c r="E9">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F9">
+        <v>1.85</v>
+      </c>
+      <c r="G9">
+        <v>1.92</v>
+      </c>
+      <c r="H9">
+        <v>0.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>